<commit_message>
Nsc [create, get single, get all , update one, delete one] Created
Create  => post nsc/
Get One => post nsc/nscId
Get ALl => get nsc/
Update one => put nsc/nscId
Delete One => delete nsc/nscId
</commit_message>
<xml_diff>
--- a/implemented_error_codes.xlsx
+++ b/implemented_error_codes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="134">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>The the number with the specified token</t>
+  </si>
+  <si>
+    <t>Succesfully created</t>
+  </si>
+  <si>
+    <t>Successfully created</t>
   </si>
 </sst>
 </file>
@@ -775,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L102" sqref="L102"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1850,6 +1856,26 @@
         <v>131</v>
       </c>
     </row>
+    <row r="104" spans="2:12">
+      <c r="B104" s="2">
+        <v>50</v>
+      </c>
+      <c r="D104" s="2">
+        <v>200</v>
+      </c>
+      <c r="F104" s="2">
+        <v>200</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>